<commit_message>
some changes to the reports and excel file
</commit_message>
<xml_diff>
--- a/results/19-Sept-2025/19-Sept-2025.xlsx
+++ b/results/19-Sept-2025/19-Sept-2025.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -23,13 +23,16 @@
     <t>Status</t>
   </si>
   <si>
-    <t>testLinksCountOnHomePage</t>
+    <t>testFileUpload</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
   <si>
     <t>testABTestingLinkNavigation</t>
   </si>
   <si>
-    <t>testFileUpload</t>
+    <t>testLinksCountOnHomePage</t>
   </si>
 </sst>
 </file>
@@ -82,6 +85,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
@@ -92,8 +101,8 @@
       <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C2" t="n" s="0">
-        <v>1.0</v>
+      <c r="C2" t="s" s="0">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -101,10 +110,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>4</v>
-      </c>
-      <c r="C3" t="n" s="0">
-        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -112,10 +121,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>1.0</v>
+      <c r="C4" t="s" s="0">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>